<commit_message>
update 4TU import to work with non-version specific DOIs, update changelog with previous fixxes in tags and new changes.
</commit_message>
<xml_diff>
--- a/storage/app/import-data/4tu/230202 4TU.RD metadata export geo_RP.xlsx
+++ b/storage/app/import-data/4tu/230202 4TU.RD metadata export geo_RP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/r_p_j_pijnenburg_uu_nl/Documents/EPOS-NL/07 Data/4TU collaboration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsh001\Projects\epos\storage\app\import-data\4tu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="14_{4B6802E5-1CAD-4BB0-AC56-A1BC54650F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B696BCBC-744C-442B-85A9-2F8003F794E5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FA5368-EE8E-49A1-A57E-C0D62A7167D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="only MSL" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2540" uniqueCount="1576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2540" uniqueCount="1621">
   <si>
     <t>doi</t>
   </si>
@@ -4766,6 +4766,141 @@
   </si>
   <si>
     <t xml:space="preserve">IF MSL --&gt; "1" </t>
+  </si>
+  <si>
+    <t>10.4121/21789452</t>
+  </si>
+  <si>
+    <t>10.4121/21678938</t>
+  </si>
+  <si>
+    <t>10.4121/21640148</t>
+  </si>
+  <si>
+    <t>10.4121/21528819</t>
+  </si>
+  <si>
+    <t>10.4121/20299644</t>
+  </si>
+  <si>
+    <t>10.4121/21523512</t>
+  </si>
+  <si>
+    <t>10.4121/21533988</t>
+  </si>
+  <si>
+    <t>10.4121/21510030</t>
+  </si>
+  <si>
+    <t>10.4121/21316563</t>
+  </si>
+  <si>
+    <t>10.4121/21187270</t>
+  </si>
+  <si>
+    <t>10.4121/15153594</t>
+  </si>
+  <si>
+    <t>10.4121/20469435</t>
+  </si>
+  <si>
+    <t>10.4121/14820342</t>
+  </si>
+  <si>
+    <t>10.4121/20179856</t>
+  </si>
+  <si>
+    <t>10.4121/19500344</t>
+  </si>
+  <si>
+    <t>10.4121/20141567</t>
+  </si>
+  <si>
+    <t>10.4121/19664427</t>
+  </si>
+  <si>
+    <t>10.4121/19519861</t>
+  </si>
+  <si>
+    <t>10.4121/12707453</t>
+  </si>
+  <si>
+    <t>10.4121/19390835</t>
+  </si>
+  <si>
+    <t>10.4121/16974109</t>
+  </si>
+  <si>
+    <t>10.4121/17121380</t>
+  </si>
+  <si>
+    <t>10.4121/17076044</t>
+  </si>
+  <si>
+    <t>10.4121/17014052</t>
+  </si>
+  <si>
+    <t>10.4121/17013755</t>
+  </si>
+  <si>
+    <t>10.4121/17004049</t>
+  </si>
+  <si>
+    <t>10.4121/16864147</t>
+  </si>
+  <si>
+    <t>10.4121/16864108</t>
+  </si>
+  <si>
+    <t>10.4121/16832254</t>
+  </si>
+  <si>
+    <t>10.4121/14464893</t>
+  </si>
+  <si>
+    <t>10.4121/16837138</t>
+  </si>
+  <si>
+    <t>10.4121/12721394</t>
+  </si>
+  <si>
+    <t>10.4121/13469325</t>
+  </si>
+  <si>
+    <t>10.4121/12852113</t>
+  </si>
+  <si>
+    <t>10.4121/16632559</t>
+  </si>
+  <si>
+    <t>10.4121/16404870</t>
+  </si>
+  <si>
+    <t>10.4121/14865096</t>
+  </si>
+  <si>
+    <t>10.4121/14537856</t>
+  </si>
+  <si>
+    <t>10.4121/14701947</t>
+  </si>
+  <si>
+    <t>10.4121/14697138</t>
+  </si>
+  <si>
+    <t>10.4121/14634021</t>
+  </si>
+  <si>
+    <t>10.4121/14619222</t>
+  </si>
+  <si>
+    <t>10.4121/14602119</t>
+  </si>
+  <si>
+    <t>10.4121/14247125</t>
+  </si>
+  <si>
+    <t>10.4121/13785643</t>
   </si>
 </sst>
 </file>
@@ -5106,20 +5241,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C8D20B-82F0-48B4-BBE4-2045E58CDA03}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="44.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="44.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.77734375" style="1"/>
-    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="44.77734375" style="1"/>
-    <col min="6" max="6" width="27.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="44.77734375" style="1"/>
+    <col min="1" max="1" width="14.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" style="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" style="1"/>
+    <col min="6" max="6" width="27.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="44.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1575</v>
       </c>
@@ -5142,12 +5279,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>1576</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -5165,12 +5302,12 @@
         <v>920</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>1577</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
@@ -5188,12 +5325,12 @@
         <v>922</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>1578</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
@@ -5211,12 +5348,12 @@
         <v>924</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>1579</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>17</v>
@@ -5234,12 +5371,12 @@
         <v>925</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>1580</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>20</v>
@@ -5257,12 +5394,12 @@
         <v>926</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>1581</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>26</v>
@@ -5280,12 +5417,12 @@
         <v>928</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>1582</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>29</v>
@@ -5303,12 +5440,12 @@
         <v>930</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>1583</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -5326,12 +5463,12 @@
         <v>932</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>1584</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -5349,12 +5486,12 @@
         <v>937</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>1585</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>48</v>
@@ -5372,12 +5509,12 @@
         <v>940</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>1586</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>51</v>
@@ -5395,12 +5532,12 @@
         <v>942</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>1587</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>54</v>
@@ -5418,12 +5555,12 @@
         <v>943</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>56</v>
+        <v>1588</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>57</v>
@@ -5441,12 +5578,12 @@
         <v>944</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>59</v>
+        <v>1589</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>60</v>
@@ -5464,12 +5601,12 @@
         <v>945</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>62</v>
+        <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>63</v>
@@ -5487,12 +5624,12 @@
         <v>946</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>65</v>
+        <v>1591</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>66</v>
@@ -5510,12 +5647,12 @@
         <v>948</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>1592</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>72</v>
@@ -5533,12 +5670,12 @@
         <v>950</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>74</v>
+        <v>1593</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>75</v>
@@ -5556,12 +5693,12 @@
         <v>952</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>77</v>
+        <v>1594</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>78</v>
@@ -5579,12 +5716,12 @@
         <v>954</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>83</v>
+        <v>1595</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>84</v>
@@ -5602,12 +5739,12 @@
         <v>957</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>89</v>
+        <v>1596</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>90</v>
@@ -5625,12 +5762,12 @@
         <v>960</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>104</v>
+        <v>1597</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>105</v>
@@ -5648,12 +5785,12 @@
         <v>968</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>107</v>
+        <v>1598</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>108</v>
@@ -5671,12 +5808,12 @@
         <v>970</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>110</v>
+        <v>1599</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>111</v>
@@ -5694,12 +5831,12 @@
         <v>971</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>113</v>
+        <v>1600</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>114</v>
@@ -5717,12 +5854,12 @@
         <v>972</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>116</v>
+        <v>1601</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>117</v>
@@ -5740,12 +5877,12 @@
         <v>973</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>119</v>
+        <v>1602</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>120</v>
@@ -5763,12 +5900,12 @@
         <v>974</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>122</v>
+        <v>1603</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>123</v>
@@ -5786,12 +5923,12 @@
         <v>974</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>125</v>
+        <v>1604</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>126</v>
@@ -5809,12 +5946,12 @@
         <v>975</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>128</v>
+        <v>1605</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>129</v>
@@ -5832,12 +5969,12 @@
         <v>976</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>131</v>
+        <v>1606</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>132</v>
@@ -5855,12 +5992,12 @@
         <v>977</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>137</v>
+        <v>1607</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>138</v>
@@ -5878,12 +6015,12 @@
         <v>980</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>1</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>143</v>
+        <v>1608</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>144</v>
@@ -5901,12 +6038,12 @@
         <v>982</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>1</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>146</v>
+        <v>1609</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>147</v>
@@ -5924,12 +6061,12 @@
         <v>984</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>1</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>149</v>
+        <v>1610</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>150</v>
@@ -5947,12 +6084,12 @@
         <v>986</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>1</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>152</v>
+        <v>1611</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>153</v>
@@ -5970,12 +6107,12 @@
         <v>987</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>1</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>173</v>
+        <v>1612</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>174</v>
@@ -5993,12 +6130,12 @@
         <v>997</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>1</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>177</v>
+        <v>1613</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>178</v>
@@ -6016,12 +6153,12 @@
         <v>998</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>1</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>180</v>
+        <v>1614</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>181</v>
@@ -6039,12 +6176,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>1</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>183</v>
+        <v>1615</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>184</v>
@@ -6062,12 +6199,12 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>1</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>186</v>
+        <v>1616</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>187</v>
@@ -6085,12 +6222,12 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>1</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>189</v>
+        <v>1617</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>190</v>
@@ -6108,12 +6245,12 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>1</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>192</v>
+        <v>1618</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>193</v>
@@ -6131,12 +6268,12 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>1</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>216</v>
+        <v>1619</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>217</v>
@@ -6154,12 +6291,12 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>1</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>243</v>
+        <v>1620</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>244</v>
@@ -6177,7 +6314,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>1</v>
       </c>
@@ -6200,7 +6337,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>1</v>
       </c>
@@ -6223,7 +6360,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>1</v>
       </c>
@@ -6246,7 +6383,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>1</v>
       </c>
@@ -6269,7 +6406,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>1</v>
       </c>
@@ -6292,7 +6429,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>1</v>
       </c>
@@ -6315,7 +6452,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>1</v>
       </c>
@@ -6338,7 +6475,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>1</v>
       </c>
@@ -6361,7 +6498,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>1</v>
       </c>
@@ -6384,7 +6521,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>1</v>
       </c>
@@ -6407,7 +6544,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>1</v>
       </c>
@@ -6430,7 +6567,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>1</v>
       </c>
@@ -6453,7 +6590,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>1</v>
       </c>
@@ -6476,7 +6613,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>1</v>
       </c>
@@ -6499,7 +6636,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>1</v>
       </c>
@@ -6522,7 +6659,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>1</v>
       </c>
@@ -6545,7 +6682,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>1</v>
       </c>
@@ -6568,7 +6705,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>1</v>
       </c>
@@ -6591,7 +6728,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>1</v>
       </c>
@@ -6614,7 +6751,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>1</v>
       </c>
@@ -6637,7 +6774,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>1</v>
       </c>
@@ -6660,7 +6797,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>1</v>
       </c>
@@ -6683,7 +6820,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>1</v>
       </c>
@@ -6706,7 +6843,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>1</v>
       </c>
@@ -6729,7 +6866,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>1</v>
       </c>
@@ -6752,7 +6889,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>1</v>
       </c>
@@ -6775,7 +6912,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>1</v>
       </c>
@@ -6798,7 +6935,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>1</v>
       </c>
@@ -6821,7 +6958,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>1</v>
       </c>
@@ -6844,7 +6981,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>1</v>
       </c>
@@ -6867,7 +7004,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>1</v>
       </c>
@@ -6890,7 +7027,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>1</v>
       </c>
@@ -6913,7 +7050,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>1</v>
       </c>
@@ -6936,7 +7073,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>1</v>
       </c>
@@ -6959,7 +7096,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>1</v>
       </c>
@@ -6982,7 +7119,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>1</v>
       </c>
@@ -7005,7 +7142,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>1</v>
       </c>
@@ -7028,7 +7165,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>1</v>
       </c>
@@ -7051,7 +7188,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>1</v>
       </c>
@@ -7074,7 +7211,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>1</v>
       </c>
@@ -7097,7 +7234,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>1</v>
       </c>
@@ -7120,7 +7257,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>1</v>
       </c>
@@ -7143,7 +7280,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>1</v>
       </c>
@@ -7166,7 +7303,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>1</v>
       </c>
@@ -7189,7 +7326,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>1</v>
       </c>
@@ -7212,7 +7349,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>1</v>
       </c>
@@ -7235,7 +7372,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>1</v>
       </c>
@@ -7258,7 +7395,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>1</v>
       </c>
@@ -7281,7 +7418,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>1</v>
       </c>
@@ -7304,7 +7441,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>1</v>
       </c>
@@ -7327,7 +7464,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>1</v>
       </c>
@@ -7350,7 +7487,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>1</v>
       </c>
@@ -7373,7 +7510,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>1</v>
       </c>
@@ -7396,7 +7533,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>1</v>
       </c>
@@ -7419,7 +7556,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>1</v>
       </c>
@@ -7458,18 +7595,18 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="44.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="44.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.77734375" style="1"/>
-    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="44.77734375" style="1"/>
-    <col min="6" max="6" width="27.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="44.77734375" style="1"/>
+    <col min="1" max="1" width="14.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" style="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" style="1"/>
+    <col min="6" max="6" width="27.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="44.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1575</v>
       </c>
@@ -7492,7 +7629,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -7515,7 +7652,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -7538,7 +7675,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -7561,7 +7698,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -7584,7 +7721,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -7607,7 +7744,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
@@ -7627,7 +7764,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -7650,7 +7787,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -7673,7 +7810,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -7696,7 +7833,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
@@ -7716,7 +7853,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>38</v>
       </c>
@@ -7736,7 +7873,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -7759,7 +7896,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>44</v>
       </c>
@@ -7779,7 +7916,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>1</v>
       </c>
@@ -7802,7 +7939,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -7825,7 +7962,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>1</v>
       </c>
@@ -7848,7 +7985,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>1</v>
       </c>
@@ -7871,7 +8008,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
@@ -7894,7 +8031,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>1</v>
       </c>
@@ -7917,7 +8054,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>1</v>
       </c>
@@ -7940,7 +8077,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>68</v>
       </c>
@@ -7960,7 +8097,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>1</v>
       </c>
@@ -7983,7 +8120,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>1</v>
       </c>
@@ -8006,7 +8143,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>1</v>
       </c>
@@ -8029,7 +8166,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>80</v>
       </c>
@@ -8049,7 +8186,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>1</v>
       </c>
@@ -8072,7 +8209,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>86</v>
       </c>
@@ -8092,7 +8229,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>1</v>
       </c>
@@ -8115,7 +8252,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>92</v>
       </c>
@@ -8135,7 +8272,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>95</v>
       </c>
@@ -8155,7 +8292,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>98</v>
       </c>
@@ -8175,7 +8312,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>101</v>
       </c>
@@ -8195,7 +8332,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>1</v>
       </c>
@@ -8218,7 +8355,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>1</v>
       </c>
@@ -8241,7 +8378,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>1</v>
       </c>
@@ -8264,7 +8401,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>1</v>
       </c>
@@ -8287,7 +8424,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>1</v>
       </c>
@@ -8310,7 +8447,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>1</v>
       </c>
@@ -8333,7 +8470,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>1</v>
       </c>
@@ -8356,7 +8493,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>1</v>
       </c>
@@ -8379,7 +8516,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>1</v>
       </c>
@@ -8402,7 +8539,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>1</v>
       </c>
@@ -8425,7 +8562,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>134</v>
       </c>
@@ -8445,7 +8582,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>1</v>
       </c>
@@ -8468,7 +8605,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>140</v>
       </c>
@@ -8488,7 +8625,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>1</v>
       </c>
@@ -8511,7 +8648,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>1</v>
       </c>
@@ -8534,7 +8671,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>1</v>
       </c>
@@ -8557,7 +8694,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>1</v>
       </c>
@@ -8580,7 +8717,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>155</v>
       </c>
@@ -8600,7 +8737,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>158</v>
       </c>
@@ -8620,7 +8757,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>161</v>
       </c>
@@ -8640,7 +8777,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>164</v>
       </c>
@@ -8660,7 +8797,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
         <v>167</v>
       </c>
@@ -8680,7 +8817,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
         <v>170</v>
       </c>
@@ -8700,7 +8837,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>1</v>
       </c>
@@ -8723,7 +8860,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>1</v>
       </c>
@@ -8746,7 +8883,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>1</v>
       </c>
@@ -8769,7 +8906,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>1</v>
       </c>
@@ -8792,7 +8929,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>1</v>
       </c>
@@ -8815,7 +8952,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>1</v>
       </c>
@@ -8838,7 +8975,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>1</v>
       </c>
@@ -8861,7 +8998,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
         <v>195</v>
       </c>
@@ -8881,7 +9018,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>198</v>
       </c>
@@ -8901,7 +9038,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>201</v>
       </c>
@@ -8921,7 +9058,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
         <v>204</v>
       </c>
@@ -8941,7 +9078,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
         <v>207</v>
       </c>
@@ -8961,7 +9098,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
         <v>210</v>
       </c>
@@ -8981,7 +9118,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
         <v>213</v>
       </c>
@@ -9001,7 +9138,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>1</v>
       </c>
@@ -9024,7 +9161,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
         <v>219</v>
       </c>
@@ -9044,7 +9181,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
         <v>222</v>
       </c>
@@ -9064,7 +9201,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
         <v>225</v>
       </c>
@@ -9084,7 +9221,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
         <v>228</v>
       </c>
@@ -9104,7 +9241,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
         <v>231</v>
       </c>
@@ -9124,7 +9261,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
         <v>234</v>
       </c>
@@ -9144,7 +9281,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
         <v>237</v>
       </c>
@@ -9164,7 +9301,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
         <v>240</v>
       </c>
@@ -9184,7 +9321,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>1</v>
       </c>
@@ -9207,7 +9344,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
         <v>246</v>
       </c>
@@ -9227,7 +9364,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
         <v>249</v>
       </c>
@@ -9247,7 +9384,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
         <v>252</v>
       </c>
@@ -9267,7 +9404,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>1</v>
       </c>
@@ -9290,7 +9427,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>1</v>
       </c>
@@ -9313,7 +9450,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>1</v>
       </c>
@@ -9336,7 +9473,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>1</v>
       </c>
@@ -9359,7 +9496,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
         <v>267</v>
       </c>
@@ -9379,7 +9516,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
         <v>270</v>
       </c>
@@ -9399,7 +9536,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>1</v>
       </c>
@@ -9422,7 +9559,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>1</v>
       </c>
@@ -9445,7 +9582,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>1</v>
       </c>
@@ -9468,7 +9605,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>1</v>
       </c>
@@ -9491,7 +9628,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
         <v>285</v>
       </c>
@@ -9511,7 +9648,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B95" s="1" t="s">
         <v>288</v>
       </c>
@@ -9531,7 +9668,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
         <v>291</v>
       </c>
@@ -9551,7 +9688,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
         <v>294</v>
       </c>
@@ -9571,7 +9708,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
         <v>297</v>
       </c>
@@ -9591,7 +9728,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>1</v>
       </c>
@@ -9614,7 +9751,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>1</v>
       </c>
@@ -9637,7 +9774,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
         <v>306</v>
       </c>
@@ -9657,7 +9794,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B102" s="1" t="s">
         <v>309</v>
       </c>
@@ -9677,7 +9814,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="s">
         <v>312</v>
       </c>
@@ -9697,7 +9834,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>1</v>
       </c>
@@ -9720,7 +9857,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="s">
         <v>318</v>
       </c>
@@ -9740,7 +9877,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
         <v>321</v>
       </c>
@@ -9760,7 +9897,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
         <v>324</v>
       </c>
@@ -9780,7 +9917,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>1</v>
       </c>
@@ -9803,7 +9940,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B109" s="1" t="s">
         <v>330</v>
       </c>
@@ -9823,7 +9960,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B110" s="1" t="s">
         <v>333</v>
       </c>
@@ -9843,7 +9980,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B111" s="1" t="s">
         <v>336</v>
       </c>
@@ -9863,7 +10000,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="s">
         <v>339</v>
       </c>
@@ -9883,7 +10020,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="s">
         <v>342</v>
       </c>
@@ -9903,7 +10040,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
         <v>345</v>
       </c>
@@ -9923,7 +10060,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="s">
         <v>348</v>
       </c>
@@ -9943,7 +10080,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="s">
         <v>351</v>
       </c>
@@ -9963,7 +10100,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
         <v>354</v>
       </c>
@@ -9983,7 +10120,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>1</v>
       </c>
@@ -10006,7 +10143,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>1</v>
       </c>
@@ -10029,7 +10166,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>1</v>
       </c>
@@ -10052,7 +10189,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B121" s="1" t="s">
         <v>366</v>
       </c>
@@ -10072,7 +10209,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>1</v>
       </c>
@@ -10095,7 +10232,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B123" s="1" t="s">
         <v>372</v>
       </c>
@@ -10115,7 +10252,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>1</v>
       </c>
@@ -10138,7 +10275,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B125" s="1" t="s">
         <v>378</v>
       </c>
@@ -10158,7 +10295,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B126" s="1" t="s">
         <v>381</v>
       </c>
@@ -10178,7 +10315,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B127" s="1" t="s">
         <v>384</v>
       </c>
@@ -10198,7 +10335,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>1</v>
       </c>
@@ -10221,7 +10358,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>1</v>
       </c>
@@ -10244,7 +10381,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B130" s="1" t="s">
         <v>392</v>
       </c>
@@ -10264,7 +10401,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B131" s="1" t="s">
         <v>395</v>
       </c>
@@ -10284,7 +10421,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="s">
         <v>398</v>
       </c>
@@ -10304,7 +10441,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B133" s="1" t="s">
         <v>400</v>
       </c>
@@ -10324,7 +10461,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B134" s="1" t="s">
         <v>403</v>
       </c>
@@ -10344,7 +10481,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>1</v>
       </c>
@@ -10367,7 +10504,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="B136" s="1" t="s">
         <v>408</v>
       </c>
@@ -10387,7 +10524,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
         <v>410</v>
       </c>
@@ -10407,7 +10544,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B138" s="1" t="s">
         <v>412</v>
       </c>
@@ -10427,7 +10564,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B139" s="1" t="s">
         <v>415</v>
       </c>
@@ -10447,7 +10584,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B140" s="1" t="s">
         <v>418</v>
       </c>
@@ -10467,7 +10604,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B141" s="1" t="s">
         <v>421</v>
       </c>
@@ -10487,7 +10624,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B142" s="1" t="s">
         <v>424</v>
       </c>
@@ -10507,7 +10644,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B143" s="1" t="s">
         <v>426</v>
       </c>
@@ -10527,7 +10664,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B144" s="1" t="s">
         <v>428</v>
       </c>
@@ -10547,7 +10684,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B145" s="1" t="s">
         <v>430</v>
       </c>
@@ -10567,7 +10704,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B146" s="1" t="s">
         <v>432</v>
       </c>
@@ -10587,7 +10724,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B147" s="1" t="s">
         <v>435</v>
       </c>
@@ -10607,7 +10744,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>1</v>
       </c>
@@ -10630,7 +10767,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B149" s="1" t="s">
         <v>441</v>
       </c>
@@ -10650,7 +10787,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B150" s="1" t="s">
         <v>444</v>
       </c>
@@ -10670,7 +10807,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B151" s="1" t="s">
         <v>447</v>
       </c>
@@ -10690,7 +10827,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B152" s="1" t="s">
         <v>450</v>
       </c>
@@ -10710,7 +10847,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>1</v>
       </c>
@@ -10733,7 +10870,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>1</v>
       </c>
@@ -10756,7 +10893,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B155" s="1" t="s">
         <v>459</v>
       </c>
@@ -10776,7 +10913,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>1</v>
       </c>
@@ -10799,7 +10936,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>1</v>
       </c>
@@ -10822,7 +10959,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>1</v>
       </c>
@@ -10845,7 +10982,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B159" s="1" t="s">
         <v>470</v>
       </c>
@@ -10865,7 +11002,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>1</v>
       </c>
@@ -10888,7 +11025,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B161" s="1" t="s">
         <v>475</v>
       </c>
@@ -10908,7 +11045,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B162" s="1" t="s">
         <v>478</v>
       </c>
@@ -10928,7 +11065,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B163" s="1" t="s">
         <v>480</v>
       </c>
@@ -10948,7 +11085,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B164" s="1" t="s">
         <v>483</v>
       </c>
@@ -10968,7 +11105,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
         <v>1</v>
       </c>
@@ -10991,7 +11128,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B166" s="1" t="s">
         <v>489</v>
       </c>
@@ -11011,7 +11148,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B167" s="1" t="s">
         <v>492</v>
       </c>
@@ -11031,7 +11168,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B168" s="1" t="s">
         <v>495</v>
       </c>
@@ -11051,7 +11188,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
         <v>1</v>
       </c>
@@ -11074,7 +11211,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B170" s="1" t="s">
         <v>500</v>
       </c>
@@ -11094,7 +11231,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B171" s="1" t="s">
         <v>503</v>
       </c>
@@ -11114,7 +11251,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B172" s="1" t="s">
         <v>506</v>
       </c>
@@ -11134,7 +11271,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B173" s="1" t="s">
         <v>508</v>
       </c>
@@ -11154,7 +11291,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
         <v>1</v>
       </c>
@@ -11177,7 +11314,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
         <v>1</v>
       </c>
@@ -11200,7 +11337,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B176" s="1" t="s">
         <v>516</v>
       </c>
@@ -11220,7 +11357,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B177" s="1" t="s">
         <v>519</v>
       </c>
@@ -11240,7 +11377,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
         <v>1</v>
       </c>
@@ -11263,7 +11400,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
         <v>1</v>
       </c>
@@ -11286,7 +11423,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B180" s="1" t="s">
         <v>528</v>
       </c>
@@ -11306,7 +11443,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B181" s="1" t="s">
         <v>531</v>
       </c>
@@ -11326,7 +11463,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B182" s="1" t="s">
         <v>533</v>
       </c>
@@ -11346,7 +11483,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B183" s="1" t="s">
         <v>535</v>
       </c>
@@ -11366,7 +11503,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B184" s="1" t="s">
         <v>538</v>
       </c>
@@ -11386,7 +11523,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B185" s="1" t="s">
         <v>541</v>
       </c>
@@ -11406,7 +11543,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B186" s="1" t="s">
         <v>544</v>
       </c>
@@ -11426,7 +11563,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="187" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B187" s="1" t="s">
         <v>547</v>
       </c>
@@ -11446,7 +11583,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B188" s="1" t="s">
         <v>550</v>
       </c>
@@ -11466,7 +11603,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B189" s="1" t="s">
         <v>552</v>
       </c>
@@ -11486,7 +11623,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="190" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B190" s="1" t="s">
         <v>555</v>
       </c>
@@ -11506,7 +11643,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B191" s="1" t="s">
         <v>558</v>
       </c>
@@ -11526,7 +11663,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="192" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B192" s="1" t="s">
         <v>561</v>
       </c>
@@ -11546,7 +11683,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B193" s="1" t="s">
         <v>564</v>
       </c>
@@ -11566,7 +11703,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="194" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B194" s="1" t="s">
         <v>567</v>
       </c>
@@ -11586,7 +11723,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="195" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A195" s="3">
         <v>1</v>
       </c>
@@ -11609,7 +11746,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="196" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B196" s="1" t="s">
         <v>572</v>
       </c>
@@ -11629,7 +11766,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B197" s="1" t="s">
         <v>575</v>
       </c>
@@ -11649,7 +11786,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="198" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B198" s="1" t="s">
         <v>577</v>
       </c>
@@ -11669,7 +11806,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="199" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B199" s="1" t="s">
         <v>580</v>
       </c>
@@ -11689,7 +11826,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="200" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A200" s="3">
         <v>1</v>
       </c>
@@ -11712,7 +11849,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="201" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A201" s="3">
         <v>1</v>
       </c>
@@ -11735,7 +11872,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="202" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B202" s="1" t="s">
         <v>589</v>
       </c>
@@ -11755,7 +11892,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="203" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B203" s="1" t="s">
         <v>591</v>
       </c>
@@ -11775,7 +11912,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="204" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A204" s="3">
         <v>1</v>
       </c>
@@ -11798,7 +11935,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="205" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A205" s="3">
         <v>1</v>
       </c>
@@ -11821,7 +11958,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="206" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B206" s="1" t="s">
         <v>599</v>
       </c>
@@ -11841,7 +11978,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="207" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B207" s="1" t="s">
         <v>602</v>
       </c>
@@ -11861,7 +11998,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="208" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A208" s="3">
         <v>1</v>
       </c>
@@ -11884,7 +12021,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="209" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A209" s="3">
         <v>1</v>
       </c>
@@ -11907,7 +12044,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="210" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B210" s="1" t="s">
         <v>611</v>
       </c>
@@ -11927,7 +12064,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="211" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B211" s="1" t="s">
         <v>613</v>
       </c>
@@ -11947,7 +12084,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="212" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B212" s="1" t="s">
         <v>616</v>
       </c>
@@ -11967,7 +12104,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="213" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B213" s="1" t="s">
         <v>619</v>
       </c>
@@ -11987,7 +12124,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B214" s="1" t="s">
         <v>622</v>
       </c>
@@ -12007,7 +12144,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A215" s="3">
         <v>1</v>
       </c>
@@ -12030,7 +12167,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="216" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B216" s="1" t="s">
         <v>628</v>
       </c>
@@ -12050,7 +12187,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="217" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B217" s="1" t="s">
         <v>631</v>
       </c>
@@ -12070,7 +12207,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="218" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B218" s="1" t="s">
         <v>633</v>
       </c>
@@ -12090,7 +12227,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="219" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B219" s="1" t="s">
         <v>636</v>
       </c>
@@ -12110,7 +12247,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="220" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B220" s="1" t="s">
         <v>639</v>
       </c>
@@ -12130,7 +12267,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="221" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B221" s="1" t="s">
         <v>642</v>
       </c>
@@ -12150,7 +12287,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="222" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B222" s="1" t="s">
         <v>644</v>
       </c>
@@ -12170,7 +12307,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A223" s="3">
         <v>1</v>
       </c>
@@ -12193,7 +12330,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="224" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A224" s="3">
         <v>1</v>
       </c>
@@ -12216,7 +12353,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="225" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B225" s="1" t="s">
         <v>653</v>
       </c>
@@ -12236,7 +12373,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="226" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" s="3">
         <v>1</v>
       </c>
@@ -12259,7 +12396,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A227" s="3">
         <v>1</v>
       </c>
@@ -12282,7 +12419,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="228" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B228" s="1" t="s">
         <v>661</v>
       </c>
@@ -12302,7 +12439,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="229" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B229" s="1" t="s">
         <v>664</v>
       </c>
@@ -12322,7 +12459,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="230" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A230" s="3">
         <v>1</v>
       </c>
@@ -12345,7 +12482,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="231" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A231" s="3">
         <v>1</v>
       </c>
@@ -12368,7 +12505,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="232" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A232" s="3">
         <v>1</v>
       </c>
@@ -12391,7 +12528,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="233" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B233" s="1" t="s">
         <v>676</v>
       </c>
@@ -12411,7 +12548,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="234" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A234" s="3">
         <v>1</v>
       </c>
@@ -12434,7 +12571,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="235" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A235" s="3">
         <v>1</v>
       </c>
@@ -12457,7 +12594,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="236" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A236" s="3">
         <v>1</v>
       </c>
@@ -12480,7 +12617,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="237" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B237" s="1" t="s">
         <v>688</v>
       </c>
@@ -12500,7 +12637,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="238" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B238" s="1" t="s">
         <v>691</v>
       </c>
@@ -12520,7 +12657,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="239" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B239" s="1" t="s">
         <v>694</v>
       </c>
@@ -12540,7 +12677,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="240" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A240" s="3">
         <v>1</v>
       </c>
@@ -12563,7 +12700,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="241" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B241" s="1" t="s">
         <v>700</v>
       </c>
@@ -12583,7 +12720,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="242" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B242" s="1" t="s">
         <v>703</v>
       </c>
@@ -12603,7 +12740,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="243" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B243" s="1" t="s">
         <v>706</v>
       </c>
@@ -12623,7 +12760,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="244" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B244" s="1" t="s">
         <v>709</v>
       </c>
@@ -12643,7 +12780,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="245" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B245" s="1" t="s">
         <v>712</v>
       </c>
@@ -12663,7 +12800,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="246" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A246" s="3">
         <v>1</v>
       </c>
@@ -12686,7 +12823,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="247" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B247" s="1" t="s">
         <v>718</v>
       </c>
@@ -12706,7 +12843,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="248" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A248" s="3">
         <v>1</v>
       </c>
@@ -12729,7 +12866,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="249" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B249" s="1" t="s">
         <v>724</v>
       </c>
@@ -12749,7 +12886,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="250" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B250" s="1" t="s">
         <v>727</v>
       </c>
@@ -12769,7 +12906,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="251" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B251" s="1" t="s">
         <v>730</v>
       </c>
@@ -12789,7 +12926,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="252" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B252" s="1" t="s">
         <v>733</v>
       </c>
@@ -12809,7 +12946,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="253" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B253" s="1" t="s">
         <v>736</v>
       </c>
@@ -12829,7 +12966,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="254" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B254" s="1" t="s">
         <v>739</v>
       </c>
@@ -12849,7 +12986,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="255" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B255" s="1" t="s">
         <v>741</v>
       </c>
@@ -12869,7 +13006,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="256" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B256" s="1" t="s">
         <v>744</v>
       </c>
@@ -12889,7 +13026,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="257" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B257" s="1" t="s">
         <v>747</v>
       </c>
@@ -12909,7 +13046,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="258" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B258" s="1" t="s">
         <v>749</v>
       </c>
@@ -12929,7 +13066,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="259" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B259" s="1" t="s">
         <v>751</v>
       </c>
@@ -12949,7 +13086,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="260" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B260" s="1" t="s">
         <v>753</v>
       </c>
@@ -12969,7 +13106,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="261" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B261" s="1" t="s">
         <v>756</v>
       </c>
@@ -12989,7 +13126,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="262" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B262" s="1" t="s">
         <v>759</v>
       </c>
@@ -13009,7 +13146,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="263" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B263" s="1" t="s">
         <v>762</v>
       </c>
@@ -13029,7 +13166,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="264" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B264" s="1" t="s">
         <v>765</v>
       </c>
@@ -13049,7 +13186,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="265" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B265" s="1" t="s">
         <v>768</v>
       </c>
@@ -13069,7 +13206,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="266" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B266" s="1" t="s">
         <v>771</v>
       </c>
@@ -13089,7 +13226,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="267" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B267" s="1" t="s">
         <v>774</v>
       </c>
@@ -13109,7 +13246,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="268" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B268" s="1" t="s">
         <v>777</v>
       </c>
@@ -13129,7 +13266,7 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="269" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A269" s="3">
         <v>1</v>
       </c>
@@ -13152,7 +13289,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="270" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B270" s="1" t="s">
         <v>783</v>
       </c>
@@ -13172,7 +13309,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="271" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B271" s="1" t="s">
         <v>786</v>
       </c>
@@ -13192,7 +13329,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="272" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B272" s="1" t="s">
         <v>789</v>
       </c>
@@ -13212,7 +13349,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="273" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="273" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B273" s="1" t="s">
         <v>792</v>
       </c>
@@ -13232,7 +13369,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="274" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="274" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B274" s="1" t="s">
         <v>795</v>
       </c>
@@ -13252,7 +13389,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="275" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="275" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B275" s="1" t="s">
         <v>798</v>
       </c>
@@ -13272,7 +13409,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="276" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="276" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B276" s="1" t="s">
         <v>801</v>
       </c>
@@ -13292,7 +13429,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="277" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="277" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B277" s="1" t="s">
         <v>804</v>
       </c>
@@ -13312,7 +13449,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="278" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="278" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B278" s="1" t="s">
         <v>808</v>
       </c>
@@ -13332,7 +13469,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="279" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="279" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B279" s="1" t="s">
         <v>811</v>
       </c>
@@ -13352,7 +13489,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="280" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="280" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B280" s="1" t="s">
         <v>814</v>
       </c>
@@ -13372,7 +13509,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="281" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="281" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B281" s="1" t="s">
         <v>817</v>
       </c>
@@ -13392,7 +13529,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="282" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="282" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B282" s="1" t="s">
         <v>819</v>
       </c>
@@ -13412,7 +13549,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="283" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="283" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B283" s="1" t="s">
         <v>821</v>
       </c>
@@ -13432,7 +13569,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="284" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="284" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B284" s="1" t="s">
         <v>823</v>
       </c>
@@ -13452,7 +13589,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="285" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="285" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B285" s="1" t="s">
         <v>825</v>
       </c>
@@ -13472,7 +13609,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="286" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="286" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B286" s="1" t="s">
         <v>827</v>
       </c>
@@ -13492,7 +13629,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="287" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="287" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B287" s="1" t="s">
         <v>829</v>
       </c>
@@ -13512,7 +13649,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="288" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="288" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B288" s="1" t="s">
         <v>831</v>
       </c>
@@ -13532,7 +13669,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="289" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="289" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B289" s="1" t="s">
         <v>833</v>
       </c>
@@ -13552,7 +13689,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="290" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="290" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B290" s="1" t="s">
         <v>835</v>
       </c>
@@ -13572,7 +13709,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="291" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="291" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B291" s="1" t="s">
         <v>838</v>
       </c>
@@ -13592,7 +13729,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="292" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="292" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B292" s="1" t="s">
         <v>841</v>
       </c>
@@ -13612,7 +13749,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="293" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="293" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B293" s="1" t="s">
         <v>844</v>
       </c>
@@ -13632,7 +13769,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="294" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="294" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B294" s="1" t="s">
         <v>847</v>
       </c>
@@ -13652,7 +13789,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="295" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="295" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B295" s="1" t="s">
         <v>850</v>
       </c>
@@ -13672,7 +13809,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="296" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="296" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B296" s="1" t="s">
         <v>853</v>
       </c>
@@ -13692,7 +13829,7 @@
         <v>1285</v>
       </c>
     </row>
-    <row r="297" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="297" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B297" s="1" t="s">
         <v>856</v>
       </c>
@@ -13712,7 +13849,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="298" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="298" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B298" s="1" t="s">
         <v>858</v>
       </c>
@@ -13732,7 +13869,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="299" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="299" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B299" s="1" t="s">
         <v>861</v>
       </c>
@@ -13752,7 +13889,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="300" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="300" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B300" s="1" t="s">
         <v>864</v>
       </c>
@@ -13772,7 +13909,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="301" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="301" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B301" s="1" t="s">
         <v>866</v>
       </c>
@@ -13792,7 +13929,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="302" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="302" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B302" s="1" t="s">
         <v>869</v>
       </c>
@@ -13812,7 +13949,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="303" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="303" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B303" s="1" t="s">
         <v>872</v>
       </c>
@@ -13832,7 +13969,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="304" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="304" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B304" s="1" t="s">
         <v>874</v>
       </c>
@@ -13852,7 +13989,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="305" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="305" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B305" s="1" t="s">
         <v>876</v>
       </c>
@@ -13872,7 +14009,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="306" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="306" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B306" s="1" t="s">
         <v>879</v>
       </c>
@@ -13892,7 +14029,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="307" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="307" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B307" s="1" t="s">
         <v>882</v>
       </c>
@@ -13912,7 +14049,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="308" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="308" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B308" s="1" t="s">
         <v>885</v>
       </c>
@@ -13932,7 +14069,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="309" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="309" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B309" s="1" t="s">
         <v>887</v>
       </c>
@@ -13952,7 +14089,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="310" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="310" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B310" s="1" t="s">
         <v>890</v>
       </c>
@@ -13972,7 +14109,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="311" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="311" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B311" s="1" t="s">
         <v>892</v>
       </c>
@@ -13992,7 +14129,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="312" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="312" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B312" s="1" t="s">
         <v>894</v>
       </c>
@@ -14012,7 +14149,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="313" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="313" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B313" s="1" t="s">
         <v>896</v>
       </c>
@@ -14032,7 +14169,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="314" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="314" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B314" s="1" t="s">
         <v>898</v>
       </c>
@@ -14052,7 +14189,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="315" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="315" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B315" s="1" t="s">
         <v>900</v>
       </c>
@@ -14072,7 +14209,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="316" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="316" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B316" s="1" t="s">
         <v>902</v>
       </c>
@@ -14092,7 +14229,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="317" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="317" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B317" s="1" t="s">
         <v>905</v>
       </c>
@@ -14112,7 +14249,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="318" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="318" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B318" s="1" t="s">
         <v>907</v>
       </c>
@@ -14132,7 +14269,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="319" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="319" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B319" s="1" t="s">
         <v>909</v>
       </c>
@@ -14152,7 +14289,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="320" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="320" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B320" s="1" t="s">
         <v>911</v>
       </c>
@@ -14172,7 +14309,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="321" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B321" s="1" t="s">
         <v>913</v>
       </c>
@@ -14192,7 +14329,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="322" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B322" s="1" t="s">
         <v>916</v>
       </c>
@@ -14212,7 +14349,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="323" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A323" s="3">
         <f>SUM(A2:A322)</f>
         <v>100</v>

</xml_diff>